<commit_message>
added autotouch scripts, script for processing solo songs, minor bugfixes
</commit_message>
<xml_diff>
--- a/data/songlist.xlsx
+++ b/data/songlist.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Desktop\ssmvp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E7503A-144D-48EB-A70B-01A31466830C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95263EDE-81C8-42C6-BE5A-477EF2F24C16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{E5388BEE-BCF6-4286-A26B-DCB9385DF1B9}"/>
   </bookViews>
   <sheets>
-    <sheet name="duos" sheetId="3" r:id="rId1"/>
-    <sheet name="songnames" sheetId="1" r:id="rId2"/>
+    <sheet name="songnames" sheetId="1" r:id="rId1"/>
+    <sheet name="duos" sheetId="3" r:id="rId2"/>
     <sheet name="songnames_alphabetical" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1536,498 +1536,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1884005B-BD56-479F-8CC6-D3ABAE97245E}">
-  <dimension ref="A1:P24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="54.5703125" customWidth="1"/>
-    <col min="7" max="7" width="52" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B1" t="s">
-        <v>373</v>
-      </c>
-      <c r="C1" t="s">
-        <v>374</v>
-      </c>
-      <c r="F1" t="str">
-        <f>$O$1&amp;"-"&amp;$P$1&amp;","&amp;"("&amp;C1&amp;"),"&amp;A1</f>
-        <v>yumi-kozue,(ORIGINAL),SONGNAME</v>
-      </c>
-      <c r="G1" t="str">
-        <f>$P$1&amp;"-"&amp;$O$1&amp;","&amp;"("&amp;C1&amp;"),"&amp;A1</f>
-        <v>kozue-yumi,(ORIGINAL),SONGNAME</v>
-      </c>
-      <c r="N1" t="s">
-        <v>375</v>
-      </c>
-      <c r="O1" t="s">
-        <v>376</v>
-      </c>
-      <c r="P1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F24" si="0">$O$1&amp;"-"&amp;$P$1&amp;","&amp;"("&amp;C2&amp;"),"&amp;A2</f>
-        <v>yumi-kozue,(Riina-Natsuki),Jet to the Future</v>
-      </c>
-      <c r="G2" t="str">
-        <f t="shared" ref="G2:G24" si="1">$P$1&amp;"-"&amp;$O$1&amp;","&amp;"("&amp;C2&amp;"),"&amp;A2</f>
-        <v>kozue-yumi,(Riina-Natsuki),Jet to the Future</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Kirari-Anzu),あんきら！？狂騒曲</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Kirari-Anzu),あんきら！？狂騒曲</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Ranko-Asuka),双翼の独奏歌</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Ranko-Asuka),双翼の独奏歌</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Rika-Mika),Twin☆くるっ★テール</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Rika-Mika),Twin☆くるっ★テール</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Syuko-Sae),美に入り彩を穿つ</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Syuko-Sae),美に入り彩を穿つ</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Rina-Takumi),Virgin Love</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Rina-Takumi),Virgin Love</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Nana-Shin),凸凹スピードスター</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Nana-Shin),凸凹スピードスター</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="3">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Shiki-Frederica),クレイジークレイジー</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Shiki-Frederica),クレイジークレイジー</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Kanade-Kaede),Pretty Liar</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Kanade-Kaede),Pretty Liar</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="3">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Koume-Ryo),アンデッド・ダンスロック</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Koume-Ryo),アンデッド・ダンスロック</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Yoshino-Hajime),Sunshine See May</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Yoshino-Hajime),Sunshine See May</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="3">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Hina-Haruna),Needle Light</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Hina-Haruna),Needle Light</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="F14" t="str">
-        <f>$O$1&amp;"-"&amp;$P$1&amp;","&amp;"("&amp;C14&amp;"),"&amp;A14</f>
-        <v>yumi-kozue,(Nagi-Hayate),O-Ku-Ri-Mo-No Sunday!</v>
-      </c>
-      <c r="G14" t="str">
-        <f>$P$1&amp;"-"&amp;$O$1&amp;","&amp;"("&amp;C14&amp;"),"&amp;A14</f>
-        <v>kozue-yumi,(Nagi-Hayate),O-Ku-Ri-Mo-No Sunday!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="3">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Shiki-Asuka),バベル</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Shiki-Asuka),バベル</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="3">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Minami-Kanade),Secret Daybreak</v>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Minami-Kanade),Secret Daybreak</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="3">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="F17" t="str">
-        <f>$O$1&amp;"-"&amp;$P$1&amp;","&amp;"("&amp;C17&amp;"),"&amp;A17</f>
-        <v>yumi-kozue,(Chitose-Chiyo),Fascinate</v>
-      </c>
-      <c r="G17" t="str">
-        <f>$P$1&amp;"-"&amp;$O$1&amp;","&amp;"("&amp;C17&amp;"),"&amp;A17</f>
-        <v>kozue-yumi,(Chitose-Chiyo),Fascinate</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="3">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Hinako-Mayu),ギュっとMilky Way</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Hinako-Mayu),ギュっとMilky Way</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="3">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Hotaru-Kako),幸せの法則 ～ルール～</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Hotaru-Kako),幸せの法則 ～ルール～</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="3">
-        <v>2</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Tomoe-Mizuki),Gaze and Gaze</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Tomoe-Mizuki),Gaze and Gaze</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="3">
-        <v>2</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Haru-Risa),輝け！ビートシューター</v>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Haru-Risa),輝け！ビートシューター</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="3">
-        <v>2</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Karin-Aiko),ほほえみDiary</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Karin-Aiko),ほほえみDiary</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="3">
-        <v>2</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Reina-Hikaru),ヒーローヴァーサスレイナンジョー</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Reina-Hikaru),ヒーローヴァーサスレイナンジョー</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>222</v>
-      </c>
-      <c r="B24" s="3">
-        <v>2</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>yumi-kozue,(Riina-Natsuki),タッタ</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="1"/>
-        <v>kozue-yumi,(Riina-Natsuki),タッタ</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE63625-E10C-4B0D-9485-4DCA2A18DC10}">
   <dimension ref="A1:C220"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
       <selection activeCell="A220" sqref="A1:C220"/>
     </sheetView>
   </sheetViews>
@@ -4685,6 +4197,494 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1884005B-BD56-479F-8CC6-D3ABAE97245E}">
+  <dimension ref="A1:P24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="54.5703125" customWidth="1"/>
+    <col min="7" max="7" width="52" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F1" t="str">
+        <f>$O$1&amp;"-"&amp;$P$1&amp;","&amp;"("&amp;C1&amp;"),"&amp;A1</f>
+        <v>yumi-kozue,(ORIGINAL),SONGNAME</v>
+      </c>
+      <c r="G1" t="str">
+        <f>$P$1&amp;"-"&amp;$O$1&amp;","&amp;"("&amp;C1&amp;"),"&amp;A1</f>
+        <v>kozue-yumi,(ORIGINAL),SONGNAME</v>
+      </c>
+      <c r="N1" t="s">
+        <v>375</v>
+      </c>
+      <c r="O1" t="s">
+        <v>376</v>
+      </c>
+      <c r="P1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F24" si="0">$O$1&amp;"-"&amp;$P$1&amp;","&amp;"("&amp;C2&amp;"),"&amp;A2</f>
+        <v>yumi-kozue,(Riina-Natsuki),Jet to the Future</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G24" si="1">$P$1&amp;"-"&amp;$O$1&amp;","&amp;"("&amp;C2&amp;"),"&amp;A2</f>
+        <v>kozue-yumi,(Riina-Natsuki),Jet to the Future</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Kirari-Anzu),あんきら！？狂騒曲</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Kirari-Anzu),あんきら！？狂騒曲</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Ranko-Asuka),双翼の独奏歌</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Ranko-Asuka),双翼の独奏歌</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Rika-Mika),Twin☆くるっ★テール</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Rika-Mika),Twin☆くるっ★テール</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Syuko-Sae),美に入り彩を穿つ</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Syuko-Sae),美に入り彩を穿つ</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Rina-Takumi),Virgin Love</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Rina-Takumi),Virgin Love</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Nana-Shin),凸凹スピードスター</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Nana-Shin),凸凹スピードスター</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Shiki-Frederica),クレイジークレイジー</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Shiki-Frederica),クレイジークレイジー</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Kanade-Kaede),Pretty Liar</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Kanade-Kaede),Pretty Liar</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Koume-Ryo),アンデッド・ダンスロック</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Koume-Ryo),アンデッド・ダンスロック</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Yoshino-Hajime),Sunshine See May</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Yoshino-Hajime),Sunshine See May</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Hina-Haruna),Needle Light</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Hina-Haruna),Needle Light</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="F14" t="str">
+        <f>$O$1&amp;"-"&amp;$P$1&amp;","&amp;"("&amp;C14&amp;"),"&amp;A14</f>
+        <v>yumi-kozue,(Nagi-Hayate),O-Ku-Ri-Mo-No Sunday!</v>
+      </c>
+      <c r="G14" t="str">
+        <f>$P$1&amp;"-"&amp;$O$1&amp;","&amp;"("&amp;C14&amp;"),"&amp;A14</f>
+        <v>kozue-yumi,(Nagi-Hayate),O-Ku-Ri-Mo-No Sunday!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Shiki-Asuka),バベル</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Shiki-Asuka),バベル</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Minami-Kanade),Secret Daybreak</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Minami-Kanade),Secret Daybreak</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="F17" t="str">
+        <f>$O$1&amp;"-"&amp;$P$1&amp;","&amp;"("&amp;C17&amp;"),"&amp;A17</f>
+        <v>yumi-kozue,(Chitose-Chiyo),Fascinate</v>
+      </c>
+      <c r="G17" t="str">
+        <f>$P$1&amp;"-"&amp;$O$1&amp;","&amp;"("&amp;C17&amp;"),"&amp;A17</f>
+        <v>kozue-yumi,(Chitose-Chiyo),Fascinate</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Hinako-Mayu),ギュっとMilky Way</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Hinako-Mayu),ギュっとMilky Way</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Hotaru-Kako),幸せの法則 ～ルール～</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Hotaru-Kako),幸せの法則 ～ルール～</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Tomoe-Mizuki),Gaze and Gaze</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Tomoe-Mizuki),Gaze and Gaze</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Haru-Risa),輝け！ビートシューター</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Haru-Risa),輝け！ビートシューター</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Karin-Aiko),ほほえみDiary</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Karin-Aiko),ほほえみDiary</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Reina-Hikaru),ヒーローヴァーサスレイナンジョー</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Reina-Hikaru),ヒーローヴァーサスレイナンジョー</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>yumi-kozue,(Riina-Natsuki),タッタ</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>kozue-yumi,(Riina-Natsuki),タッタ</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97DE646-2E7B-4156-9338-DB11927BE8AD}">
   <dimension ref="A1:B220"/>

</xml_diff>